<commit_message>
[0.4.0.1] prep trad integration
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/Input Sheet.xlsx
+++ b/IRCS2-devbuild/source/Input Sheet.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. IRCS Automation\Control 2 DEV\IRCS-v2\IRCS2-devbuild\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EE7030-3858-4197-8B5A-5A7AC092D022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A107C-C4A7-4C52-A0FA-D48D0E500607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
   </bookViews>
   <sheets>
     <sheet name="PATH INPUT" sheetId="7" r:id="rId1"/>
     <sheet name="CODE LIBRARY" sheetId="1" r:id="rId2"/>
     <sheet name="&gt;&gt;&gt;" sheetId="2" r:id="rId3"/>
     <sheet name="UL" sheetId="5" r:id="rId4"/>
-    <sheet name="TRAD" sheetId="4" r:id="rId5"/>
-    <sheet name="SPEC" sheetId="6" r:id="rId6"/>
+    <sheet name="SPEC UL" sheetId="6" r:id="rId5"/>
+    <sheet name="TRAD" sheetId="8" r:id="rId6"/>
+    <sheet name="SPEC TRAD" sheetId="9" r:id="rId7"/>
+    <sheet name="Campaign Lookup" sheetId="10" r:id="rId8"/>
+    <sheet name="Code BSI" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">UL!$A$1:$B$151</definedName>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="484">
   <si>
     <t>Prophet Code</t>
   </si>
@@ -835,9 +838,6 @@
     <t>CSAMAN</t>
   </si>
   <si>
-    <t>MYWAR</t>
-  </si>
-  <si>
     <t>CSGREN</t>
   </si>
   <si>
@@ -1433,13 +1433,79 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>CTSL__A</t>
+  </si>
+  <si>
+    <t>MJG1</t>
+  </si>
+  <si>
+    <t>MJG2</t>
+  </si>
+  <si>
+    <t>RIDTCIAS</t>
+  </si>
+  <si>
+    <t>RID_HCPTM</t>
+  </si>
+  <si>
+    <t>RID_PB77A3</t>
+  </si>
+  <si>
+    <t>RID_PB77</t>
+  </si>
+  <si>
+    <t>Campaign Type</t>
+  </si>
+  <si>
+    <t>Curr</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Max Bonus</t>
+  </si>
+  <si>
+    <t>IDR</t>
+  </si>
+  <si>
+    <t>1_IDR</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>1_USD</t>
+  </si>
+  <si>
+    <t>2_IDR</t>
+  </si>
+  <si>
+    <t>2_USD</t>
+  </si>
+  <si>
+    <t>3_IDR</t>
+  </si>
+  <si>
+    <t>Cover_code</t>
+  </si>
+  <si>
+    <t>Grouping raw data</t>
+  </si>
+  <si>
+    <t>SPKTAMBSI</t>
+  </si>
+  <si>
+    <t>SPKTAPBSI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1574,31 +1640,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1773,8 +1843,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B1D2F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1904,6 +1998,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1912,52 +2017,55 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2003,78 +2111,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2406,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA018573-BF85-417A-8309-CECE2ACCAF79}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" activeCellId="1" sqref="B6 J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,50 +2454,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -2619,7 +2656,7 @@
     </row>
     <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -2675,7 +2712,7 @@
     </row>
     <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -2691,7 +2728,7 @@
     </row>
     <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -2731,7 +2768,7 @@
     </row>
     <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -2947,10 +2984,10 @@
     </row>
     <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>265</v>
+      </c>
+      <c r="B55" t="s">
         <v>266</v>
-      </c>
-      <c r="B55" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3163,7 +3200,7 @@
     </row>
     <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B82" t="s">
         <v>170</v>
@@ -3195,7 +3232,7 @@
     </row>
     <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B86" t="s">
         <v>39</v>
@@ -3211,7 +3248,7 @@
     </row>
     <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B88" t="s">
         <v>140</v>
@@ -3403,7 +3440,7 @@
     </row>
     <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B112" t="s">
         <v>152</v>
@@ -3515,7 +3552,7 @@
     </row>
     <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B126" t="s">
         <v>179</v>
@@ -3539,7 +3576,7 @@
     </row>
     <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B129" t="s">
         <v>179</v>
@@ -3555,7 +3592,7 @@
     </row>
     <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B131" t="s">
         <v>179</v>
@@ -3603,7 +3640,7 @@
     </row>
     <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B137" t="s">
         <v>195</v>
@@ -3734,854 +3771,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FE0483-7A79-4679-AE77-EC53F6C33D68}">
-  <dimension ref="B1:C102"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B91" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B93" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>431</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B73:B90 C91:C98">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83:B84">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B85:B90 C91:C98">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B100:B101">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C73:C90 B91:B98">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C83:C90 B91:B98">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 Internal&amp;1#_x000D_</oddHeader>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6501272E-EDEF-4543-BBF4-AA0015E04FA3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -4593,15 +3782,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" t="s">
         <v>444</v>
-      </c>
-      <c r="B1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B2" t="s">
         <v>199</v>
@@ -4609,7 +3798,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -4617,7 +3806,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B4" t="s">
         <v>140</v>
@@ -4625,7 +3814,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -4633,10 +3822,1062 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B6" t="s">
         <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A3CEDA-FEC6-4ADF-A8A7-FE3D173EF629}">
+  <dimension ref="A1:B102"/>
+  <sheetViews>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="6"/>
+      <c r="B102" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB54F92-38AE-4ECD-91DC-DF9206C91F4C}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB1AC11-73D5-4AD4-B5BC-7F2393CC7475}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" s="6">
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="D4" s="6">
+        <v>500000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="D5" s="6">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="D6" s="6">
+        <v>100000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AEBD3E-E17A-4FD7-BDAF-3A1BA4999487}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[0.4.0.4] minor bug fix
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/Input Sheet.xlsx
+++ b/IRCS2-devbuild/source/Input Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. IRCS Automation\Control 2 DEV\IRCS-v2\IRCS2-devbuild\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CF1F2A-95DA-44EC-B1EA-78F8D468BD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2858EE52-F052-4738-AA31-6702CABAE5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="488">
   <si>
     <t>Prophet Code</t>
   </si>
@@ -1505,6 +1505,12 @@
   </si>
   <si>
     <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>LGC_LGM_Campaign</t>
+  </si>
+  <si>
+    <t>D:\1. IRCS Automation\Source\IRCS2\LGC &amp; LGM Campaign\LGC_LGM_Campaign_Mar25.txt</t>
   </si>
 </sst>
 </file>
@@ -2447,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA018573-BF85-417A-8309-CECE2ACCAF79}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2508,9 +2514,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>454</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>461</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[0.4.1.7] input sheet update
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/Input Sheet.xlsx
+++ b/IRCS2-devbuild/source/Input Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. IRCS Automation\Control 2 DEV\IRCS-v2\IRCS2-devbuild\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8DEE34-33C9-43B2-B91E-C2817A940A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B23330-A4A8-46E8-86F7-82E504979BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
   </bookViews>
   <sheets>
     <sheet name="PATH INPUT" sheetId="7" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="496">
   <si>
     <t>Prophet Code</t>
   </si>
@@ -1519,9 +1519,6 @@
     <t>D:\1. IRCS Automation\Source\IRCS2\LGC &amp; LGM Campaign\BSI_ATTRIBUSI_020425.xlsx</t>
   </si>
   <si>
-    <t>Reporting Period</t>
-  </si>
-  <si>
     <t>RESERVE_TRADCONV_RWNB_IFRS_2025</t>
   </si>
   <si>
@@ -1532,13 +1529,19 @@
   </si>
   <si>
     <t>D:\1. IRCS Automation\Source\IRCS2\LGC &amp; LGM Campaign\RESERVE_TRADSHA_RWNB_IFRS_20250402.txt</t>
+  </si>
+  <si>
+    <t>Reporting Quarter</t>
+  </si>
+  <si>
+    <t>Financial Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1695,8 +1698,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1900,6 +1911,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -2087,7 +2104,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2099,6 +2116,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2474,110 +2494,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA018573-BF85-417A-8309-CECE2ACCAF79}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>490</v>
-      </c>
-      <c r="B2">
+        <v>494</v>
+      </c>
+      <c r="B2" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>450</v>
-      </c>
-      <c r="B3" t="s">
-        <v>458</v>
+        <v>495</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2025</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>451</v>
-      </c>
-      <c r="B4" t="s">
-        <v>457</v>
+        <v>450</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>453</v>
-      </c>
-      <c r="B5" t="s">
-        <v>459</v>
+        <v>451</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>452</v>
-      </c>
-      <c r="B6" t="s">
-        <v>460</v>
+        <v>453</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>485</v>
-      </c>
-      <c r="B7" t="s">
-        <v>484</v>
+        <v>452</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>486</v>
-      </c>
-      <c r="B8" t="s">
-        <v>487</v>
+        <v>485</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>488</v>
-      </c>
-      <c r="B9" t="s">
-        <v>489</v>
+        <v>486</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>491</v>
-      </c>
-      <c r="B10" t="s">
-        <v>493</v>
+        <v>488</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>490</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>492</v>
-      </c>
-      <c r="B11" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>491</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>454</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="9" t="s">
         <v>461</v>
       </c>
     </row>
@@ -2588,12 +2617,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF0FC1C-2639-4C1B-AF6A-FF06FADA9C91}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 Internal&amp;1#_x000D_</oddHeader>
@@ -2603,6 +2689,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126961A8-B58E-4CDB-9B7C-33D17EC49D0F}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4931,7 +5020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AEBD3E-E17A-4FD7-BDAF-3A1BA4999487}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>